<commit_message>
updated configurations for each mapping
</commit_message>
<xml_diff>
--- a/codelists.xlsx
+++ b/codelists.xlsx
@@ -241,12 +241,145 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="F120">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Purchasing Group: "X99"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F83">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "25"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F79">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "21"
+	-Sofia Perova
+we should have a list of everything that was filtered out for the validation
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F78">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "20"
+	-Sofia Perova</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B78">
       <text>
         <t xml:space="preserve">@gennie.nguyen@portlandoregon.gov
 	-Sofia Perova
 Exclude IGA and Grant
+	-Gennie Nguyen
+Should we filter out from publication those records that have Type Code values IGA and Grant?
+	-Sofia Perova</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="F39">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "25"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F35">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "21"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F34">
+      <text>
+        <t xml:space="preserve">should be filtered out from publication Type Code: "20"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B13">
+      <text>
+        <t xml:space="preserve">@sofia.perova@quintagroup.org The list includes deprecated codes for the version of the standard we are applying. They are included in the documentation because some publishers are still using older versions, but they should not be used in our case.
+I recommend changing 'lowestCost' to 'costOnly'
+'bestProposal' to 'relatedCriteria.'
+"bestProposal" to "relatedCriteria"
+	-Félix Penna
+@fpenna@open-contracting.org replaced "lowestCost" with "costOnly"
+	-Sofia Perova</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G39">
+      <text>
+        <t xml:space="preserve">@gennie.nguyen@portlandoregon.gov
+	-Sofia Perova
+There is a subset of data that is grouped together. Rather than identifying the procurements like the others, Procurement decided to tag them as "Housing Emergency." The emergency has ended. The recommend matching looking at the SAP Contract Listing Report or the SAP PO Listing Report to identify the appropriate type_code for this field as "G&amp;S," "PTE" or "Construction." Then the second part of the type_code should be "Emergency."
+	-Gennie Nguyen
+We need to map this type to one of the existing awardCriteria values: 
+- costOnly
+- ratedCriteria
+- lowestCost
+- priceOnly
+	-Sofia Perova
+Can filter out and flag for review?
 	-Gennie Nguyen</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G35">
+      <text>
+        <t xml:space="preserve">@gennie.nguyen@portlandoregon.gov
+	-Sofia Perova
+There's only one line when I sort for type_code = 21. I checked with the supervisor, and the selection is user error. All type_code = 21 is an error and requires review.
+	-Gennie Nguyen
+We need to map this type to one of the existing awardCriteria values: 
+- costOnly
+- ratedCriteria
+- lowestCost
+- priceOnly
+	-Sofia Perova
+Can we filter out and flag for review?
+	-Gennie Nguyen</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G34">
+      <text>
+        <t xml:space="preserve">@gennie.nguyen@portlandoregon.gov
+	-Sofia Perova
+There is only one type_code =21 in the entire dataset. I checked with the supervisor, and this is user error. All selections for type_code = 21 requires review.
+	-Gennie Nguyen
+We need to map this type to one of the existing awardCriteria values: 
+- costOnly
+- ratedCriteria
+- lowestCost
+- priceOnly
+	-Sofia Perova
+Can we filter out and flag for review?
+	-Gennie Nguyen</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G27">
+      <text>
+        <t xml:space="preserve">@gennie.nguyen@portlandoregon.gov
+	-Sofia Perova
+RFQ = Request for Qualifications which is request for information. Procurement puts out an RFQ to gather information access how many and which vendors are in the market, especially in cases when our specifications are very specific. It helps us decide if we want to award a sole source, for example. In other cases, Procurement may use it as market research. A PTE RFQ may be followed by an RFP or QBS RFP.
+	-Gennie Nguyen
+We need to map this type to one of the existing awardCriteria values: 
+- costOnly
+- ratedCriteria
+- lowestCost
+- priceOnly
+	-Sofia Perova
+RFQs don't result in an award.
+	-Gennie Nguyen
+@gennie.nguyen@portlandoregon.gov does this mean that we should filter out from publication all records that have Type Code = PTE RFQ?
+	-Sofia Perova</t>
       </text>
     </comment>
   </commentList>
@@ -254,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="1884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4657" uniqueCount="1883">
   <si>
     <t>Codelist Mapping Template</t>
   </si>
@@ -5997,6 +6130,9 @@
     <t xml:space="preserve">sofia.perova@quintagroup.org- Looking in the entire dataset, no type_code: 18 exists. </t>
   </si>
   <si>
+    <t>null</t>
+  </si>
+  <si>
     <t xml:space="preserve">sofia.perova@quintagroup.org- Looking at the entire dataset, one requisition came up: 131565 (bid #2335). The procurement agent used this as an announcement on bid posting on BuySpeed, and does not count as a procurement project. I will make this option "inactive" in BuySpeed. Requisition #131565 (bid#2335) should be excluded from the dataset. </t>
   </si>
   <si>
@@ -6131,12 +6267,6 @@
   </si>
   <si>
     <t>The award will be made to the qualified bid demonstrating the highest score against a set of weighted criteria such as price, cost and quality (including, for example, the environmental and social impact of the procurement). Structured information on individual qualifying criteria can be provided with the requirements extension.</t>
-  </si>
-  <si>
-    <t>lowestCost</t>
-  </si>
-  <si>
-    <t>Lowest cost</t>
   </si>
   <si>
     <t>This code has been deprecated. Please choose from one of the other codes.</t>
@@ -7388,7 +7518,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7498,6 +7628,9 @@
     <font>
       <color rgb="FF333333"/>
       <name val="&quot;DejaVu Sans&quot;"/>
+    </font>
+    <font>
+      <strike/>
     </font>
     <font>
       <b/>
@@ -7736,7 +7869,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="97">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7997,13 +8130,27 @@
     <xf borderId="19" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -23213,13 +23360,13 @@
         <v>21</v>
       </c>
       <c r="B78" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C78" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D78" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E78" s="82" t="s">
         <v>523</v>
@@ -23232,7 +23379,7 @@
         <v>IGA</v>
       </c>
       <c r="H78" s="84" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="I78" s="86"/>
     </row>
@@ -23241,13 +23388,13 @@
         <v>21</v>
       </c>
       <c r="B79" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C79" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D79" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E79" s="82" t="s">
         <v>523</v>
@@ -23260,7 +23407,7 @@
         <v>Grant</v>
       </c>
       <c r="H79" s="84" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="I79" s="87"/>
     </row>
@@ -23344,13 +23491,13 @@
         <v>21</v>
       </c>
       <c r="B83" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C83" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D83" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E83" s="82" t="s">
         <v>523</v>
@@ -23363,7 +23510,7 @@
         <v>Housing Emergency</v>
       </c>
       <c r="H83" s="84" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="84">
@@ -24270,14 +24417,14 @@
       <c r="A120" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B120" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="C120" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="D120" s="16" t="s">
-        <v>296</v>
+      <c r="B120" s="85" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C120" s="85" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D120" s="85" t="s">
+        <v>1422</v>
       </c>
       <c r="E120" s="82" t="s">
         <v>699</v>
@@ -24301,7 +24448,7 @@
         <v>1324</v>
       </c>
       <c r="B122" s="77" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="123">
@@ -24335,13 +24482,13 @@
         <v>21</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="C124" s="16" t="s">
         <v>400</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="E124" s="79"/>
       <c r="F124" s="82"/>
@@ -24362,7 +24509,7 @@
         <v>388</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="E125" s="82" t="s">
         <v>505</v>
@@ -24384,7 +24531,7 @@
         <v>388</v>
       </c>
       <c r="D126" s="16" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="E126" s="82" t="s">
         <v>505</v>
@@ -24409,7 +24556,7 @@
         <v>388</v>
       </c>
       <c r="D127" s="16" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="E127" s="82" t="s">
         <v>505</v>
@@ -24434,7 +24581,7 @@
         <v>1392</v>
       </c>
       <c r="D128" s="16" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="E128" s="82" t="s">
         <v>505</v>
@@ -24459,7 +24606,7 @@
         <v>1395</v>
       </c>
       <c r="D129" s="16" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="E129" s="79"/>
       <c r="F129" s="79"/>
@@ -24479,7 +24626,7 @@
         <v>1324</v>
       </c>
       <c r="B131" s="77" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="132">
@@ -24513,13 +24660,13 @@
         <v>21</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="C133" s="16" t="s">
         <v>400</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="E133" s="79"/>
       <c r="F133" s="79"/>
@@ -24540,7 +24687,7 @@
         <v>388</v>
       </c>
       <c r="D134" s="16" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="E134" s="79"/>
       <c r="F134" s="79"/>
@@ -24561,7 +24708,7 @@
         <v>1392</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="E135" s="79"/>
       <c r="F135" s="79"/>
@@ -24576,13 +24723,13 @@
         <v>21</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="E136" s="79"/>
       <c r="F136" s="79"/>
@@ -24602,7 +24749,7 @@
         <v>1324</v>
       </c>
       <c r="B138" s="77" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="139">
@@ -24636,13 +24783,13 @@
         <v>21</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D140" s="16" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="E140" s="79"/>
       <c r="F140" s="79"/>
@@ -24657,13 +24804,13 @@
         <v>21</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D141" s="16" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="E141" s="79"/>
       <c r="F141" s="79"/>
@@ -24678,13 +24825,13 @@
         <v>21</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D142" s="16" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="E142" s="79"/>
       <c r="F142" s="79"/>
@@ -24699,13 +24846,13 @@
         <v>21</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D143" s="16" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="E143" s="79"/>
       <c r="F143" s="79"/>
@@ -24773,7 +24920,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="2">
@@ -24781,7 +24928,7 @@
         <v>1318</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="3">
@@ -24810,7 +24957,7 @@
         <v>1324</v>
       </c>
       <c r="B6" s="77" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="7">
@@ -24850,7 +24997,7 @@
         <v>1418</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="79"/>
@@ -24871,7 +25018,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="79"/>
@@ -24892,7 +25039,7 @@
         <v>560</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="E10" s="79"/>
       <c r="F10" s="79"/>
@@ -24907,13 +25054,13 @@
         <v>21</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="E11" s="79"/>
       <c r="F11" s="79"/>
@@ -24933,7 +25080,7 @@
         <v>1324</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="14">
@@ -24967,13 +25114,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E15" s="82" t="s">
         <v>523</v>
@@ -24992,13 +25139,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E16" s="82" t="s">
         <v>523</v>
@@ -25017,13 +25164,13 @@
         <v>21</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>1468</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>1469</v>
       </c>
       <c r="E17" s="82" t="s">
         <v>523</v>
@@ -25042,13 +25189,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E18" s="82" t="s">
         <v>523</v>
@@ -25067,13 +25214,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E19" s="82" t="s">
         <v>523</v>
@@ -25092,13 +25239,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E20" s="82" t="s">
         <v>523</v>
@@ -25117,13 +25264,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>1470</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>1471</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>1472</v>
       </c>
       <c r="E21" s="82" t="s">
         <v>523</v>
@@ -25142,13 +25289,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E22" s="82" t="s">
         <v>523</v>
@@ -25167,14 +25314,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D23" s="16"/>
       <c r="E23" s="82" t="s">
         <v>523</v>
       </c>
@@ -25192,14 +25337,12 @@
         <v>21</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D24" s="16"/>
       <c r="E24" s="82" t="s">
         <v>523</v>
       </c>
@@ -25217,13 +25360,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E25" s="82" t="s">
         <v>523</v>
@@ -25242,13 +25385,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E26" s="82" t="s">
         <v>523</v>
@@ -25266,14 +25409,14 @@
       <c r="A27" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="85" t="s">
-        <v>296</v>
-      </c>
-      <c r="C27" s="85" t="s">
-        <v>296</v>
-      </c>
-      <c r="D27" s="85" t="s">
-        <v>296</v>
+      <c r="B27" s="16" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>1467</v>
       </c>
       <c r="E27" s="82" t="s">
         <v>523</v>
@@ -25292,13 +25435,13 @@
         <v>21</v>
       </c>
       <c r="B28" s="16" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>1473</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="D28" s="16" t="s">
         <v>1474</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>1475</v>
       </c>
       <c r="E28" s="82" t="s">
         <v>523</v>
@@ -25317,13 +25460,13 @@
         <v>21</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C29" s="16" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>1468</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>1469</v>
       </c>
       <c r="E29" s="82" t="s">
         <v>523</v>
@@ -25342,13 +25485,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>1470</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>1471</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>1472</v>
       </c>
       <c r="E30" s="82" t="s">
         <v>523</v>
@@ -25367,14 +25510,12 @@
         <v>21</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D31" s="16"/>
       <c r="E31" s="82" t="s">
         <v>523</v>
       </c>
@@ -25392,14 +25533,12 @@
         <v>21</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="82" t="s">
         <v>523</v>
       </c>
@@ -25417,13 +25556,13 @@
         <v>21</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E33" s="82" t="s">
         <v>523</v>
@@ -25442,13 +25581,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D34" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E34" s="82" t="s">
         <v>523</v>
@@ -25467,13 +25606,13 @@
         <v>21</v>
       </c>
       <c r="B35" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D35" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E35" s="82" t="s">
         <v>523</v>
@@ -25492,13 +25631,13 @@
         <v>21</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E36" s="82" t="s">
         <v>523</v>
@@ -25517,13 +25656,13 @@
         <v>21</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E37" s="82" t="s">
         <v>523</v>
@@ -25542,13 +25681,13 @@
         <v>21</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E38" s="82" t="s">
         <v>523</v>
@@ -25567,13 +25706,13 @@
         <v>21</v>
       </c>
       <c r="B39" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="D39" s="85" t="s">
-        <v>296</v>
+        <v>1422</v>
       </c>
       <c r="E39" s="82" t="s">
         <v>523</v>
@@ -25592,13 +25731,13 @@
         <v>21</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E40" s="82" t="s">
         <v>523</v>
@@ -25617,13 +25756,13 @@
         <v>21</v>
       </c>
       <c r="B41" s="16" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>1470</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="D41" s="16" t="s">
         <v>1471</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>1472</v>
       </c>
       <c r="E41" s="82" t="s">
         <v>461</v>
@@ -25642,13 +25781,13 @@
         <v>21</v>
       </c>
       <c r="B42" s="16" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>1470</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="D42" s="16" t="s">
         <v>1471</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>1472</v>
       </c>
       <c r="E42" s="82" t="s">
         <v>461</v>
@@ -25667,13 +25806,13 @@
         <v>21</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E43" s="82" t="s">
         <v>461</v>
@@ -25692,13 +25831,13 @@
         <v>21</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E44" s="82" t="s">
         <v>461</v>
@@ -25717,13 +25856,13 @@
         <v>21</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E45" s="82" t="s">
         <v>461</v>
@@ -25742,13 +25881,13 @@
         <v>21</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E46" s="82" t="s">
         <v>461</v>
@@ -25767,13 +25906,13 @@
         <v>21</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E47" s="82" t="s">
         <v>461</v>
@@ -25792,13 +25931,13 @@
         <v>21</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E48" s="82" t="s">
         <v>461</v>
@@ -25817,13 +25956,13 @@
         <v>21</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E49" s="82" t="s">
         <v>461</v>
@@ -25842,13 +25981,13 @@
         <v>21</v>
       </c>
       <c r="B50" s="16" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>1473</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="D50" s="16" t="s">
         <v>1474</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>1475</v>
       </c>
       <c r="E50" s="82" t="s">
         <v>461</v>
@@ -25867,13 +26006,13 @@
         <v>21</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E51" s="82" t="s">
         <v>461</v>
@@ -25892,13 +26031,13 @@
         <v>21</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E52" s="82" t="s">
         <v>461</v>
@@ -25917,13 +26056,13 @@
         <v>21</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E53" s="82" t="s">
         <v>461</v>
@@ -25942,13 +26081,13 @@
         <v>21</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E54" s="82" t="s">
         <v>461</v>
@@ -25967,13 +26106,13 @@
         <v>21</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E55" s="82" t="s">
         <v>461</v>
@@ -25992,13 +26131,13 @@
         <v>21</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E56" s="82" t="s">
         <v>461</v>
@@ -26017,13 +26156,13 @@
         <v>21</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E57" s="82" t="s">
         <v>461</v>
@@ -26042,14 +26181,12 @@
         <v>21</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D58" s="16"/>
       <c r="E58" s="82" t="s">
         <v>461</v>
       </c>
@@ -26067,14 +26204,12 @@
         <v>21</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D59" s="16"/>
       <c r="E59" s="82" t="s">
         <v>461</v>
       </c>
@@ -26092,14 +26227,12 @@
         <v>21</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D60" s="16"/>
       <c r="E60" s="82" t="s">
         <v>461</v>
       </c>
@@ -26117,14 +26250,12 @@
         <v>21</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D61" s="16"/>
       <c r="E61" s="82" t="s">
         <v>461</v>
       </c>
@@ -26142,14 +26273,12 @@
         <v>21</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D62" s="16"/>
       <c r="E62" s="82" t="s">
         <v>461</v>
       </c>
@@ -26167,14 +26296,12 @@
         <v>21</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D63" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D63" s="16"/>
       <c r="E63" s="82" t="s">
         <v>461</v>
       </c>
@@ -26192,14 +26319,12 @@
         <v>21</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>1469</v>
-      </c>
+        <v>1463</v>
+      </c>
+      <c r="D64" s="16"/>
       <c r="E64" s="82" t="s">
         <v>461</v>
       </c>
@@ -26213,67 +26338,119 @@
       <c r="H64" s="81"/>
     </row>
     <row r="65">
-      <c r="A65" s="74" t="s">
+      <c r="A65" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="89" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C65" s="89" t="s">
         <v>1476</v>
       </c>
-      <c r="C65" s="16" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E65" s="79"/>
-      <c r="F65" s="79"/>
-      <c r="G65" s="80" t="str">
+      <c r="D65" s="89"/>
+      <c r="E65" s="90"/>
+      <c r="F65" s="90"/>
+      <c r="G65" s="91" t="str">
         <f>IFERROR(VLOOKUP(CONCATENATE(E65,F65),'(Source) Codelists'!$D:$F,3,FALSE))</f>
         <v/>
       </c>
-      <c r="H65" s="81"/>
+      <c r="H65" s="92"/>
+      <c r="I65" s="93"/>
+      <c r="J65" s="93"/>
+      <c r="K65" s="93"/>
+      <c r="L65" s="93"/>
+      <c r="M65" s="93"/>
+      <c r="N65" s="93"/>
+      <c r="O65" s="93"/>
+      <c r="P65" s="93"/>
+      <c r="Q65" s="93"/>
+      <c r="R65" s="93"/>
+      <c r="S65" s="93"/>
+      <c r="T65" s="93"/>
+      <c r="U65" s="93"/>
+      <c r="V65" s="93"/>
+      <c r="W65" s="93"/>
+      <c r="X65" s="93"/>
+      <c r="Y65" s="93"/>
+      <c r="Z65" s="93"/>
     </row>
     <row r="66">
-      <c r="A66" s="74" t="s">
+      <c r="A66" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="89" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C66" s="89" t="s">
         <v>1478</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="D66" s="89" t="s">
         <v>1479</v>
       </c>
-      <c r="D66" s="16" t="s">
-        <v>1480</v>
-      </c>
-      <c r="E66" s="79"/>
-      <c r="F66" s="79"/>
-      <c r="G66" s="80" t="str">
+      <c r="E66" s="90"/>
+      <c r="F66" s="90"/>
+      <c r="G66" s="91" t="str">
         <f>IFERROR(VLOOKUP(CONCATENATE(E66,F66),'(Source) Codelists'!$D:$F,3,FALSE))</f>
         <v/>
       </c>
-      <c r="H66" s="81"/>
+      <c r="H66" s="92"/>
+      <c r="I66" s="93"/>
+      <c r="J66" s="93"/>
+      <c r="K66" s="93"/>
+      <c r="L66" s="93"/>
+      <c r="M66" s="93"/>
+      <c r="N66" s="93"/>
+      <c r="O66" s="93"/>
+      <c r="P66" s="93"/>
+      <c r="Q66" s="93"/>
+      <c r="R66" s="93"/>
+      <c r="S66" s="93"/>
+      <c r="T66" s="93"/>
+      <c r="U66" s="93"/>
+      <c r="V66" s="93"/>
+      <c r="W66" s="93"/>
+      <c r="X66" s="93"/>
+      <c r="Y66" s="93"/>
+      <c r="Z66" s="93"/>
     </row>
     <row r="67">
-      <c r="A67" s="74" t="s">
+      <c r="A67" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="89" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C67" s="89" t="s">
         <v>1481</v>
       </c>
-      <c r="C67" s="16" t="s">
-        <v>1482</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E67" s="79"/>
-      <c r="F67" s="79"/>
-      <c r="G67" s="80" t="str">
+      <c r="D67" s="89" t="s">
+        <v>1468</v>
+      </c>
+      <c r="E67" s="90"/>
+      <c r="F67" s="90"/>
+      <c r="G67" s="91" t="str">
         <f>IFERROR(VLOOKUP(CONCATENATE(E67,F67),'(Source) Codelists'!$D:$F,3,FALSE))</f>
         <v/>
       </c>
-      <c r="H67" s="81"/>
+      <c r="H67" s="92"/>
+      <c r="I67" s="93"/>
+      <c r="J67" s="93"/>
+      <c r="K67" s="93"/>
+      <c r="L67" s="93"/>
+      <c r="M67" s="93"/>
+      <c r="N67" s="93"/>
+      <c r="O67" s="93"/>
+      <c r="P67" s="93"/>
+      <c r="Q67" s="93"/>
+      <c r="R67" s="93"/>
+      <c r="S67" s="93"/>
+      <c r="T67" s="93"/>
+      <c r="U67" s="93"/>
+      <c r="V67" s="93"/>
+      <c r="W67" s="93"/>
+      <c r="X67" s="93"/>
+      <c r="Y67" s="93"/>
+      <c r="Z67" s="93"/>
     </row>
     <row r="68">
       <c r="A68" s="74" t="s">
@@ -26285,7 +26462,7 @@
         <v>1324</v>
       </c>
       <c r="B69" s="77" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="70">
@@ -26319,13 +26496,13 @@
         <v>21</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>1484</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="D71" s="16" t="s">
         <v>1485</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>1486</v>
       </c>
       <c r="E71" s="79"/>
       <c r="F71" s="79"/>
@@ -26340,13 +26517,13 @@
         <v>21</v>
       </c>
       <c r="B72" s="16" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>1487</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="D72" s="16" t="s">
         <v>1488</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>1489</v>
       </c>
       <c r="E72" s="79"/>
       <c r="F72" s="79"/>
@@ -26361,13 +26538,13 @@
         <v>21</v>
       </c>
       <c r="B73" s="16" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C73" s="16" t="s">
         <v>1490</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="D73" s="16" t="s">
         <v>1491</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>1492</v>
       </c>
       <c r="E73" s="79"/>
       <c r="F73" s="79"/>
@@ -26382,13 +26559,13 @@
         <v>21</v>
       </c>
       <c r="B74" s="16" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C74" s="16" t="s">
         <v>1493</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="D74" s="16" t="s">
         <v>1494</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>1495</v>
       </c>
       <c r="E74" s="79"/>
       <c r="F74" s="79"/>
@@ -26408,7 +26585,7 @@
         <v>1324</v>
       </c>
       <c r="B76" s="77" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="77">
@@ -26442,13 +26619,13 @@
         <v>21</v>
       </c>
       <c r="B78" s="16" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C78" s="16" t="s">
         <v>1497</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="D78" s="16" t="s">
         <v>1498</v>
-      </c>
-      <c r="D78" s="16" t="s">
-        <v>1499</v>
       </c>
       <c r="E78" s="79"/>
       <c r="F78" s="79"/>
@@ -26463,13 +26640,13 @@
         <v>21</v>
       </c>
       <c r="B79" s="16" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C79" s="16" t="s">
         <v>1500</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>1501</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>1502</v>
       </c>
       <c r="E79" s="79"/>
       <c r="F79" s="79"/>
@@ -26484,13 +26661,13 @@
         <v>21</v>
       </c>
       <c r="B80" s="16" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C80" s="16" t="s">
         <v>1503</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="D80" s="16" t="s">
         <v>1504</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>1505</v>
       </c>
       <c r="E80" s="79"/>
       <c r="F80" s="79"/>
@@ -26505,13 +26682,13 @@
         <v>21</v>
       </c>
       <c r="B81" s="16" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C81" s="16" t="s">
         <v>1506</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="D81" s="16" t="s">
         <v>1507</v>
-      </c>
-      <c r="D81" s="16" t="s">
-        <v>1508</v>
       </c>
       <c r="E81" s="79"/>
       <c r="F81" s="79"/>
@@ -26526,13 +26703,13 @@
         <v>21</v>
       </c>
       <c r="B82" s="16" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C82" s="16" t="s">
         <v>1509</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="D82" s="16" t="s">
         <v>1510</v>
-      </c>
-      <c r="D82" s="16" t="s">
-        <v>1511</v>
       </c>
       <c r="E82" s="79"/>
       <c r="F82" s="79"/>
@@ -26547,13 +26724,13 @@
         <v>21</v>
       </c>
       <c r="B83" s="16" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C83" s="16" t="s">
         <v>1512</v>
       </c>
-      <c r="C83" s="16" t="s">
+      <c r="D83" s="16" t="s">
         <v>1513</v>
-      </c>
-      <c r="D83" s="16" t="s">
-        <v>1514</v>
       </c>
       <c r="E83" s="79"/>
       <c r="F83" s="79"/>
@@ -26568,13 +26745,13 @@
         <v>21</v>
       </c>
       <c r="B84" s="16" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C84" s="16" t="s">
         <v>1515</v>
       </c>
-      <c r="C84" s="16" t="s">
+      <c r="D84" s="16" t="s">
         <v>1516</v>
-      </c>
-      <c r="D84" s="16" t="s">
-        <v>1517</v>
       </c>
       <c r="E84" s="79"/>
       <c r="F84" s="79"/>
@@ -26589,13 +26766,13 @@
         <v>21</v>
       </c>
       <c r="B85" s="16" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C85" s="16" t="s">
         <v>1518</v>
       </c>
-      <c r="C85" s="16" t="s">
+      <c r="D85" s="16" t="s">
         <v>1519</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>1520</v>
       </c>
       <c r="E85" s="79"/>
       <c r="F85" s="79"/>
@@ -26615,7 +26792,7 @@
         <v>1324</v>
       </c>
       <c r="B87" s="77" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="88">
@@ -26649,13 +26826,13 @@
         <v>21</v>
       </c>
       <c r="B89" s="16" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C89" s="16" t="s">
         <v>1522</v>
       </c>
-      <c r="C89" s="16" t="s">
+      <c r="D89" s="16" t="s">
         <v>1523</v>
-      </c>
-      <c r="D89" s="16" t="s">
-        <v>1524</v>
       </c>
       <c r="E89" s="79"/>
       <c r="F89" s="79"/>
@@ -26670,13 +26847,13 @@
         <v>21</v>
       </c>
       <c r="B90" s="16" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C90" s="16" t="s">
         <v>1525</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="D90" s="16" t="s">
         <v>1526</v>
-      </c>
-      <c r="D90" s="16" t="s">
-        <v>1527</v>
       </c>
       <c r="E90" s="79"/>
       <c r="F90" s="79"/>
@@ -26691,13 +26868,13 @@
         <v>21</v>
       </c>
       <c r="B91" s="16" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C91" s="16" t="s">
         <v>1528</v>
       </c>
-      <c r="C91" s="16" t="s">
+      <c r="D91" s="16" t="s">
         <v>1529</v>
-      </c>
-      <c r="D91" s="16" t="s">
-        <v>1530</v>
       </c>
       <c r="E91" s="79"/>
       <c r="F91" s="79"/>
@@ -26712,13 +26889,13 @@
         <v>21</v>
       </c>
       <c r="B92" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C92" s="16" t="s">
         <v>1531</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="D92" s="16" t="s">
         <v>1532</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>1533</v>
       </c>
       <c r="E92" s="79"/>
       <c r="F92" s="79"/>
@@ -26733,13 +26910,13 @@
         <v>21</v>
       </c>
       <c r="B93" s="16" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C93" s="16" t="s">
         <v>1534</v>
       </c>
-      <c r="C93" s="16" t="s">
+      <c r="D93" s="16" t="s">
         <v>1535</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>1536</v>
       </c>
       <c r="E93" s="79"/>
       <c r="F93" s="79"/>
@@ -26754,13 +26931,13 @@
         <v>21</v>
       </c>
       <c r="B94" s="16" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C94" s="16" t="s">
         <v>1537</v>
       </c>
-      <c r="C94" s="16" t="s">
+      <c r="D94" s="16" t="s">
         <v>1538</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>1539</v>
       </c>
       <c r="E94" s="79"/>
       <c r="F94" s="79"/>
@@ -26775,13 +26952,13 @@
         <v>21</v>
       </c>
       <c r="B95" s="16" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C95" s="16" t="s">
         <v>1540</v>
       </c>
-      <c r="C95" s="16" t="s">
+      <c r="D95" s="16" t="s">
         <v>1541</v>
-      </c>
-      <c r="D95" s="16" t="s">
-        <v>1542</v>
       </c>
       <c r="E95" s="79"/>
       <c r="F95" s="79"/>
@@ -26796,13 +26973,13 @@
         <v>21</v>
       </c>
       <c r="B96" s="16" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C96" s="16" t="s">
         <v>1543</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="D96" s="16" t="s">
         <v>1544</v>
-      </c>
-      <c r="D96" s="16" t="s">
-        <v>1545</v>
       </c>
       <c r="E96" s="79"/>
       <c r="F96" s="79"/>
@@ -26817,13 +26994,13 @@
         <v>21</v>
       </c>
       <c r="B97" s="16" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C97" s="16" t="s">
         <v>1546</v>
       </c>
-      <c r="C97" s="16" t="s">
+      <c r="D97" s="16" t="s">
         <v>1547</v>
-      </c>
-      <c r="D97" s="16" t="s">
-        <v>1548</v>
       </c>
       <c r="E97" s="79"/>
       <c r="F97" s="79"/>
@@ -26838,13 +27015,13 @@
         <v>21</v>
       </c>
       <c r="B98" s="16" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C98" s="16" t="s">
         <v>1549</v>
       </c>
-      <c r="C98" s="16" t="s">
+      <c r="D98" s="16" t="s">
         <v>1550</v>
-      </c>
-      <c r="D98" s="16" t="s">
-        <v>1551</v>
       </c>
       <c r="E98" s="79"/>
       <c r="F98" s="79"/>
@@ -26864,7 +27041,7 @@
         <v>1324</v>
       </c>
       <c r="B100" s="77" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="101">
@@ -26898,13 +27075,13 @@
         <v>21</v>
       </c>
       <c r="B102" s="16" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C102" s="16" t="s">
         <v>1553</v>
       </c>
-      <c r="C102" s="16" t="s">
+      <c r="D102" s="16" t="s">
         <v>1554</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>1555</v>
       </c>
       <c r="E102" s="79"/>
       <c r="F102" s="79"/>
@@ -26919,13 +27096,13 @@
         <v>21</v>
       </c>
       <c r="B103" s="16" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C103" s="16" t="s">
         <v>1556</v>
       </c>
-      <c r="C103" s="16" t="s">
+      <c r="D103" s="16" t="s">
         <v>1557</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>1558</v>
       </c>
       <c r="E103" s="79"/>
       <c r="F103" s="79"/>
@@ -26940,13 +27117,13 @@
         <v>21</v>
       </c>
       <c r="B104" s="16" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C104" s="16" t="s">
         <v>1559</v>
       </c>
-      <c r="C104" s="16" t="s">
+      <c r="D104" s="16" t="s">
         <v>1560</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>1561</v>
       </c>
       <c r="E104" s="79"/>
       <c r="F104" s="79"/>
@@ -26961,13 +27138,13 @@
         <v>21</v>
       </c>
       <c r="B105" s="16" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C105" s="16" t="s">
         <v>1562</v>
       </c>
-      <c r="C105" s="16" t="s">
+      <c r="D105" s="16" t="s">
         <v>1563</v>
-      </c>
-      <c r="D105" s="16" t="s">
-        <v>1564</v>
       </c>
       <c r="E105" s="79"/>
       <c r="F105" s="79"/>
@@ -26982,13 +27159,13 @@
         <v>21</v>
       </c>
       <c r="B106" s="16" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C106" s="16" t="s">
         <v>1565</v>
       </c>
-      <c r="C106" s="16" t="s">
+      <c r="D106" s="16" t="s">
         <v>1566</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>1567</v>
       </c>
       <c r="E106" s="79"/>
       <c r="F106" s="79"/>
@@ -27003,13 +27180,13 @@
         <v>21</v>
       </c>
       <c r="B107" s="16" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C107" s="16" t="s">
         <v>1568</v>
       </c>
-      <c r="C107" s="16" t="s">
+      <c r="D107" s="16" t="s">
         <v>1569</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>1570</v>
       </c>
       <c r="E107" s="79"/>
       <c r="F107" s="79"/>
@@ -27024,13 +27201,13 @@
         <v>21</v>
       </c>
       <c r="B108" s="16" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C108" s="16" t="s">
         <v>1571</v>
       </c>
-      <c r="C108" s="16" t="s">
+      <c r="D108" s="16" t="s">
         <v>1572</v>
-      </c>
-      <c r="D108" s="16" t="s">
-        <v>1573</v>
       </c>
       <c r="E108" s="79"/>
       <c r="F108" s="79"/>
@@ -27045,13 +27222,13 @@
         <v>21</v>
       </c>
       <c r="B109" s="16" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C109" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="D109" s="16" t="s">
         <v>1575</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>1576</v>
       </c>
       <c r="E109" s="79"/>
       <c r="F109" s="79"/>
@@ -27066,13 +27243,13 @@
         <v>21</v>
       </c>
       <c r="B110" s="16" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C110" s="16" t="s">
         <v>1577</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="D110" s="16" t="s">
         <v>1578</v>
-      </c>
-      <c r="D110" s="16" t="s">
-        <v>1579</v>
       </c>
       <c r="E110" s="79"/>
       <c r="F110" s="79"/>
@@ -27087,13 +27264,13 @@
         <v>21</v>
       </c>
       <c r="B111" s="16" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C111" s="16" t="s">
         <v>1580</v>
       </c>
-      <c r="C111" s="16" t="s">
+      <c r="D111" s="16" t="s">
         <v>1581</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>1582</v>
       </c>
       <c r="E111" s="79"/>
       <c r="F111" s="79"/>
@@ -27108,13 +27285,13 @@
         <v>21</v>
       </c>
       <c r="B112" s="16" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C112" s="16" t="s">
         <v>1583</v>
       </c>
-      <c r="C112" s="16" t="s">
+      <c r="D112" s="16" t="s">
         <v>1584</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>1585</v>
       </c>
       <c r="E112" s="79"/>
       <c r="F112" s="79"/>
@@ -27134,7 +27311,7 @@
         <v>1324</v>
       </c>
       <c r="B114" s="77" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="115">
@@ -27168,13 +27345,13 @@
         <v>21</v>
       </c>
       <c r="B116" s="16" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C116" s="16" t="s">
         <v>1587</v>
       </c>
-      <c r="C116" s="16" t="s">
+      <c r="D116" s="16" t="s">
         <v>1588</v>
-      </c>
-      <c r="D116" s="16" t="s">
-        <v>1589</v>
       </c>
       <c r="E116" s="79"/>
       <c r="F116" s="79"/>
@@ -27192,10 +27369,10 @@
         <v>1334</v>
       </c>
       <c r="C117" s="16" t="s">
+        <v>1589</v>
+      </c>
+      <c r="D117" s="16" t="s">
         <v>1590</v>
-      </c>
-      <c r="D117" s="16" t="s">
-        <v>1591</v>
       </c>
       <c r="E117" s="79"/>
       <c r="F117" s="79"/>
@@ -27210,13 +27387,13 @@
         <v>21</v>
       </c>
       <c r="B118" s="16" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C118" s="16" t="s">
         <v>1592</v>
       </c>
-      <c r="C118" s="16" t="s">
+      <c r="D118" s="16" t="s">
         <v>1593</v>
-      </c>
-      <c r="D118" s="16" t="s">
-        <v>1594</v>
       </c>
       <c r="E118" s="79"/>
       <c r="F118" s="79"/>
@@ -27231,13 +27408,13 @@
         <v>21</v>
       </c>
       <c r="B119" s="16" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C119" s="16" t="s">
         <v>1595</v>
       </c>
-      <c r="C119" s="16" t="s">
+      <c r="D119" s="16" t="s">
         <v>1596</v>
-      </c>
-      <c r="D119" s="16" t="s">
-        <v>1597</v>
       </c>
       <c r="E119" s="79"/>
       <c r="F119" s="79"/>
@@ -27252,13 +27429,13 @@
         <v>21</v>
       </c>
       <c r="B120" s="16" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C120" s="16" t="s">
         <v>1598</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="D120" s="16" t="s">
         <v>1599</v>
-      </c>
-      <c r="D120" s="16" t="s">
-        <v>1600</v>
       </c>
       <c r="E120" s="79"/>
       <c r="F120" s="79"/>
@@ -27273,13 +27450,13 @@
         <v>21</v>
       </c>
       <c r="B121" s="16" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C121" s="16" t="s">
         <v>1601</v>
       </c>
-      <c r="C121" s="16" t="s">
+      <c r="D121" s="16" t="s">
         <v>1602</v>
-      </c>
-      <c r="D121" s="16" t="s">
-        <v>1603</v>
       </c>
       <c r="E121" s="79"/>
       <c r="F121" s="79"/>
@@ -27294,13 +27471,13 @@
         <v>21</v>
       </c>
       <c r="B122" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C122" s="16" t="s">
         <v>1604</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="D122" s="16" t="s">
         <v>1605</v>
-      </c>
-      <c r="D122" s="16" t="s">
-        <v>1606</v>
       </c>
       <c r="E122" s="79"/>
       <c r="F122" s="79"/>
@@ -27315,13 +27492,13 @@
         <v>21</v>
       </c>
       <c r="B123" s="16" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C123" s="16" t="s">
         <v>1607</v>
       </c>
-      <c r="C123" s="16" t="s">
+      <c r="D123" s="16" t="s">
         <v>1608</v>
-      </c>
-      <c r="D123" s="16" t="s">
-        <v>1609</v>
       </c>
       <c r="E123" s="79"/>
       <c r="F123" s="79"/>
@@ -27341,7 +27518,7 @@
         <v>1324</v>
       </c>
       <c r="B125" s="77" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="126">
@@ -27375,13 +27552,13 @@
         <v>21</v>
       </c>
       <c r="B127" s="16" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C127" s="16" t="s">
         <v>1611</v>
       </c>
-      <c r="C127" s="16" t="s">
+      <c r="D127" s="16" t="s">
         <v>1612</v>
-      </c>
-      <c r="D127" s="16" t="s">
-        <v>1613</v>
       </c>
       <c r="E127" s="79"/>
       <c r="F127" s="79"/>
@@ -27414,7 +27591,8 @@
       <formula1>'(Source) Codelists'!$C$5:$C$591</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -27441,7 +27619,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="2">
@@ -27449,7 +27627,7 @@
         <v>1318</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="3">
@@ -27478,7 +27656,7 @@
         <v>1324</v>
       </c>
       <c r="B6" s="77" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="7">
@@ -27486,10 +27664,10 @@
         <v>1326</v>
       </c>
       <c r="B7" s="78" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C7" s="78" t="s">
         <v>1617</v>
-      </c>
-      <c r="C7" s="78" t="s">
-        <v>1618</v>
       </c>
       <c r="D7" s="78" t="s">
         <v>1327</v>
@@ -27517,18 +27695,18 @@
       <c r="A8" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="88"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>1619</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>1620</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>1621</v>
       </c>
       <c r="G8" s="79"/>
       <c r="H8" s="79"/>
@@ -27543,19 +27721,19 @@
         <v>21</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D9" s="16" t="s">
+        <v>1622</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>1623</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>1624</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>1625</v>
       </c>
       <c r="G9" s="79"/>
       <c r="H9" s="79"/>
@@ -27570,19 +27748,19 @@
         <v>21</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>1352</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>1626</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>1627</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>1628</v>
       </c>
       <c r="G10" s="79"/>
       <c r="H10" s="79"/>
@@ -27597,19 +27775,19 @@
         <v>21</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>1361</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>1628</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>1629</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>1630</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>1631</v>
       </c>
       <c r="G11" s="79"/>
       <c r="H11" s="79"/>
@@ -27624,19 +27802,19 @@
         <v>21</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>1370</v>
       </c>
       <c r="D12" s="16" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>1632</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>1633</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>1634</v>
       </c>
       <c r="G12" s="79"/>
       <c r="H12" s="79"/>
@@ -27651,19 +27829,19 @@
         <v>21</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D13" s="16" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>1635</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>1636</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>1637</v>
       </c>
       <c r="G13" s="79"/>
       <c r="H13" s="79"/>
@@ -27678,19 +27856,19 @@
         <v>21</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D14" s="16" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>1638</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="16" t="s">
         <v>1639</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>1640</v>
       </c>
       <c r="G14" s="79"/>
       <c r="H14" s="79"/>
@@ -27705,19 +27883,19 @@
         <v>21</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D15" s="16" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>1641</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="16" t="s">
         <v>1642</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>1643</v>
       </c>
       <c r="G15" s="79"/>
       <c r="H15" s="79"/>
@@ -27732,19 +27910,19 @@
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>1644</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>1645</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>1646</v>
       </c>
       <c r="G16" s="79"/>
       <c r="H16" s="79"/>
@@ -27759,19 +27937,19 @@
         <v>21</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D17" s="16" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>1648</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="16" t="s">
         <v>1649</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>1650</v>
       </c>
       <c r="G17" s="79"/>
       <c r="H17" s="79"/>
@@ -27786,19 +27964,19 @@
         <v>21</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>1651</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>1652</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>1653</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>1654</v>
       </c>
       <c r="G18" s="79"/>
       <c r="H18" s="79"/>
@@ -27813,19 +27991,19 @@
         <v>21</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>1361</v>
       </c>
       <c r="D19" s="16" t="s">
+        <v>1654</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>1655</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>1656</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>1657</v>
       </c>
       <c r="G19" s="79"/>
       <c r="H19" s="79"/>
@@ -27840,19 +28018,19 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>1658</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>1659</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>1660</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>1661</v>
       </c>
       <c r="G20" s="79"/>
       <c r="H20" s="79"/>
@@ -27867,19 +28045,19 @@
         <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D21" s="16" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>1662</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>1663</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>1664</v>
       </c>
       <c r="G21" s="79"/>
       <c r="H21" s="79"/>
@@ -27894,19 +28072,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>1370</v>
       </c>
       <c r="D22" s="16" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>1665</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="F22" s="16" t="s">
         <v>1666</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>1667</v>
       </c>
       <c r="G22" s="79"/>
       <c r="H22" s="79"/>
@@ -27921,19 +28099,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>1370</v>
       </c>
       <c r="D23" s="16" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>1668</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="F23" s="16" t="s">
         <v>1669</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>1670</v>
       </c>
       <c r="G23" s="79"/>
       <c r="H23" s="79"/>
@@ -27948,19 +28126,19 @@
         <v>21</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>1370</v>
       </c>
       <c r="D24" s="16" t="s">
+        <v>1670</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>1671</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="F24" s="16" t="s">
         <v>1672</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>1673</v>
       </c>
       <c r="G24" s="79"/>
       <c r="H24" s="79"/>
@@ -27975,19 +28153,19 @@
         <v>21</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D25" s="16" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>1674</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="F25" s="16" t="s">
         <v>1675</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>1676</v>
       </c>
       <c r="G25" s="79"/>
       <c r="H25" s="79"/>
@@ -28002,19 +28180,19 @@
         <v>21</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D26" s="16" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>1677</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="F26" s="16" t="s">
         <v>1678</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>1679</v>
       </c>
       <c r="G26" s="79"/>
       <c r="H26" s="79"/>
@@ -28029,19 +28207,19 @@
         <v>21</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D27" s="16" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E27" s="16" t="s">
         <v>1680</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="16" t="s">
         <v>1681</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>1682</v>
       </c>
       <c r="G27" s="79"/>
       <c r="H27" s="79"/>
@@ -28056,19 +28234,19 @@
         <v>21</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D28" s="16" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>1683</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="F28" s="16" t="s">
         <v>1684</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>1685</v>
       </c>
       <c r="G28" s="79"/>
       <c r="H28" s="79"/>
@@ -28083,19 +28261,19 @@
         <v>21</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D29" s="16" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>1686</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="F29" s="16" t="s">
         <v>1687</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>1688</v>
       </c>
       <c r="G29" s="79"/>
       <c r="H29" s="79"/>
@@ -28110,19 +28288,19 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>1689</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>1690</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>1691</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="F30" s="16" t="s">
         <v>1692</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>1693</v>
       </c>
       <c r="G30" s="79"/>
       <c r="H30" s="79"/>
@@ -28137,19 +28315,19 @@
         <v>21</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D31" s="16" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>1694</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="F31" s="16" t="s">
         <v>1695</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>1696</v>
       </c>
       <c r="G31" s="79"/>
       <c r="H31" s="79"/>
@@ -28164,19 +28342,19 @@
         <v>21</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D32" s="16" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>1697</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="F32" s="16" t="s">
         <v>1698</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>1699</v>
       </c>
       <c r="G32" s="79"/>
       <c r="H32" s="79"/>
@@ -28191,19 +28369,19 @@
         <v>21</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>1352</v>
       </c>
       <c r="D33" s="16" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>1700</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="F33" s="16" t="s">
         <v>1701</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>1702</v>
       </c>
       <c r="G33" s="79"/>
       <c r="H33" s="79"/>
@@ -28218,19 +28396,19 @@
         <v>21</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D34" s="16" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>1703</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="F34" s="16" t="s">
         <v>1704</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>1705</v>
       </c>
       <c r="G34" s="79"/>
       <c r="H34" s="79"/>
@@ -28245,19 +28423,19 @@
         <v>21</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>1361</v>
       </c>
       <c r="D35" s="16" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>1706</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>1707</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>1708</v>
       </c>
       <c r="G35" s="79"/>
       <c r="H35" s="79"/>
@@ -28272,19 +28450,19 @@
         <v>21</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C36" s="16" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>1709</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="E36" s="16" t="s">
         <v>1710</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="F36" s="16" t="s">
         <v>1711</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>1712</v>
       </c>
       <c r="G36" s="79"/>
       <c r="H36" s="79"/>
@@ -28299,19 +28477,19 @@
         <v>21</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>1361</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="E37" s="16" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>1713</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>1714</v>
       </c>
       <c r="G37" s="79"/>
       <c r="H37" s="79"/>
@@ -28326,19 +28504,19 @@
         <v>21</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D38" s="16" t="s">
+        <v>1714</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>1715</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="F38" s="16" t="s">
         <v>1716</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>1717</v>
       </c>
       <c r="G38" s="79"/>
       <c r="H38" s="79"/>
@@ -28353,19 +28531,19 @@
         <v>21</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D39" s="16" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>1718</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="F39" s="16" t="s">
         <v>1719</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>1720</v>
       </c>
       <c r="G39" s="79"/>
       <c r="H39" s="79"/>
@@ -28380,19 +28558,19 @@
         <v>21</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>1334</v>
       </c>
       <c r="D40" s="16" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E40" s="16" t="s">
         <v>1721</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="F40" s="16" t="s">
         <v>1722</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>1723</v>
       </c>
       <c r="G40" s="79"/>
       <c r="H40" s="79"/>
@@ -28407,19 +28585,19 @@
         <v>21</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>1340</v>
       </c>
       <c r="D41" s="16" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>1724</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="F41" s="16" t="s">
         <v>1725</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>1726</v>
       </c>
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
@@ -28434,19 +28612,19 @@
         <v>21</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C42" s="16" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>1727</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>1728</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="F42" s="16" t="s">
         <v>1729</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>1730</v>
       </c>
       <c r="G42" s="79"/>
       <c r="H42" s="79"/>
@@ -28461,19 +28639,19 @@
         <v>21</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C43" s="16" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>1731</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>1732</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="F43" s="16" t="s">
         <v>1733</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>1734</v>
       </c>
       <c r="G43" s="79"/>
       <c r="H43" s="79"/>
@@ -28488,19 +28666,19 @@
         <v>21</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>1370</v>
       </c>
       <c r="D44" s="16" t="s">
+        <v>1734</v>
+      </c>
+      <c r="E44" s="16" t="s">
         <v>1735</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="F44" s="16" t="s">
         <v>1736</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>1737</v>
       </c>
       <c r="G44" s="79"/>
       <c r="H44" s="79"/>
@@ -28515,19 +28693,19 @@
         <v>21</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C45" s="16" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D45" s="16" t="s">
         <v>1738</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E45" s="16" t="s">
         <v>1739</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="F45" s="16" t="s">
         <v>1740</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>1741</v>
       </c>
       <c r="G45" s="79"/>
       <c r="H45" s="79"/>
@@ -28542,19 +28720,19 @@
         <v>21</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C46" s="16" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D46" s="16" t="s">
         <v>1742</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="E46" s="16" t="s">
         <v>1743</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="F46" s="16" t="s">
         <v>1744</v>
-      </c>
-      <c r="F46" s="16" t="s">
-        <v>1745</v>
       </c>
       <c r="G46" s="79"/>
       <c r="H46" s="79"/>
@@ -28569,19 +28747,19 @@
         <v>21</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>1361</v>
       </c>
       <c r="D47" s="16" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>1746</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="F47" s="16" t="s">
         <v>1747</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>1748</v>
       </c>
       <c r="G47" s="79"/>
       <c r="H47" s="79"/>
@@ -28596,19 +28774,19 @@
         <v>21</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D48" s="16" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>1749</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="16" t="s">
         <v>1750</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>1751</v>
       </c>
       <c r="G48" s="79"/>
       <c r="H48" s="79"/>
@@ -28661,7 +28839,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="2">
@@ -28669,7 +28847,7 @@
         <v>1318</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="3">
@@ -28685,7 +28863,7 @@
         <v>1318</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="5">
@@ -28711,18 +28889,18 @@
     </row>
     <row r="8">
       <c r="A8" s="74" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B8" s="95" t="s">
         <v>1755</v>
-      </c>
-      <c r="B8" s="89" t="s">
-        <v>1756</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="74" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B9" s="96" t="s">
         <v>1757</v>
-      </c>
-      <c r="B9" s="90" t="s">
-        <v>1758</v>
       </c>
     </row>
     <row r="10">
@@ -28735,7 +28913,7 @@
         <v>1324</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="12">
@@ -28769,13 +28947,13 @@
         <v>21</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>1760</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>1761</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>1762</v>
       </c>
       <c r="E13" s="79"/>
       <c r="F13" s="79"/>
@@ -28790,13 +28968,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>1763</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>1764</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>1765</v>
       </c>
       <c r="E14" s="79"/>
       <c r="F14" s="79"/>
@@ -28811,13 +28989,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="16" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>1766</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>1767</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>1768</v>
       </c>
       <c r="E15" s="79"/>
       <c r="F15" s="79"/>
@@ -28832,13 +29010,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>1769</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>1770</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>1771</v>
       </c>
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
@@ -28853,13 +29031,13 @@
         <v>21</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>1772</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>1773</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>1774</v>
       </c>
       <c r="E17" s="79"/>
       <c r="F17" s="79"/>
@@ -28874,13 +29052,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>1774</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>1775</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>1776</v>
       </c>
       <c r="E18" s="79"/>
       <c r="F18" s="79"/>
@@ -28895,13 +29073,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="16" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>1777</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>1778</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>1779</v>
       </c>
       <c r="E19" s="79"/>
       <c r="F19" s="79"/>
@@ -28916,13 +29094,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>1780</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>1781</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>1782</v>
       </c>
       <c r="E20" s="79"/>
       <c r="F20" s="79"/>
@@ -28937,13 +29115,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>1783</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>1784</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>1785</v>
       </c>
       <c r="E21" s="79"/>
       <c r="F21" s="79"/>
@@ -28958,13 +29136,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>1786</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>1787</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>1788</v>
       </c>
       <c r="E22" s="79"/>
       <c r="F22" s="79"/>
@@ -28979,13 +29157,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>1789</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>1790</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>1791</v>
       </c>
       <c r="E23" s="79"/>
       <c r="F23" s="79"/>
@@ -29000,13 +29178,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>1792</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D24" s="16" t="s">
         <v>1793</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>1794</v>
       </c>
       <c r="E24" s="79"/>
       <c r="F24" s="79"/>
@@ -29021,13 +29199,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>1795</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="D25" s="16" t="s">
         <v>1796</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>1797</v>
       </c>
       <c r="E25" s="79"/>
       <c r="F25" s="79"/>
@@ -29042,13 +29220,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="16" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>1798</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="D26" s="16" t="s">
         <v>1799</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>1800</v>
       </c>
       <c r="E26" s="79"/>
       <c r="F26" s="79"/>
@@ -29068,7 +29246,7 @@
         <v>1324</v>
       </c>
       <c r="B28" s="77" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="29">
@@ -29102,13 +29280,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>1802</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>1803</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>1804</v>
       </c>
       <c r="E30" s="79"/>
       <c r="F30" s="79"/>
@@ -29123,13 +29301,13 @@
         <v>21</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>400</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="E31" s="79"/>
       <c r="F31" s="79"/>
@@ -29144,13 +29322,13 @@
         <v>21</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>1806</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>1807</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>1808</v>
       </c>
       <c r="E32" s="79"/>
       <c r="F32" s="79"/>
@@ -29165,13 +29343,13 @@
         <v>21</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>1809</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>1810</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>1811</v>
       </c>
       <c r="E33" s="79"/>
       <c r="F33" s="79"/>
@@ -29192,7 +29370,7 @@
         <v>402</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="E34" s="79"/>
       <c r="F34" s="79"/>
@@ -29209,18 +29387,18 @@
     </row>
     <row r="36">
       <c r="A36" s="74" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B36" s="89" t="s">
-        <v>1813</v>
+        <v>1754</v>
+      </c>
+      <c r="B36" s="95" t="s">
+        <v>1812</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="74" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B37" s="90" t="s">
-        <v>1814</v>
+        <v>1756</v>
+      </c>
+      <c r="B37" s="96" t="s">
+        <v>1813</v>
       </c>
     </row>
     <row r="38">
@@ -29233,7 +29411,7 @@
         <v>1324</v>
       </c>
       <c r="B39" s="77" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="40">
@@ -29267,13 +29445,13 @@
         <v>21</v>
       </c>
       <c r="B41" s="16" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>1537</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>1538</v>
-      </c>
       <c r="D41" s="16" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="E41" s="79"/>
       <c r="F41" s="79"/>
@@ -29290,18 +29468,18 @@
     </row>
     <row r="43">
       <c r="A43" s="74" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B43" s="89" t="s">
-        <v>1816</v>
+        <v>1754</v>
+      </c>
+      <c r="B43" s="95" t="s">
+        <v>1815</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="74" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B44" s="90" t="s">
-        <v>1817</v>
+        <v>1756</v>
+      </c>
+      <c r="B44" s="96" t="s">
+        <v>1816</v>
       </c>
     </row>
     <row r="45">
@@ -29314,7 +29492,7 @@
         <v>1324</v>
       </c>
       <c r="B46" s="77" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="47">
@@ -29348,13 +29526,13 @@
         <v>21</v>
       </c>
       <c r="B48" s="16" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>1819</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="D48" s="16" t="s">
         <v>1820</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>1821</v>
       </c>
       <c r="E48" s="79"/>
       <c r="F48" s="79"/>
@@ -29369,13 +29547,13 @@
         <v>21</v>
       </c>
       <c r="B49" s="16" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>1822</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>1823</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>1824</v>
       </c>
       <c r="E49" s="79"/>
       <c r="F49" s="79"/>
@@ -29390,13 +29568,13 @@
         <v>21</v>
       </c>
       <c r="B50" s="16" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>1825</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="D50" s="16" t="s">
         <v>1826</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>1827</v>
       </c>
       <c r="E50" s="79"/>
       <c r="F50" s="79"/>
@@ -29411,13 +29589,13 @@
         <v>21</v>
       </c>
       <c r="B51" s="16" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C51" s="16" t="s">
         <v>1828</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="D51" s="16" t="s">
         <v>1829</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>1830</v>
       </c>
       <c r="E51" s="79"/>
       <c r="F51" s="79"/>
@@ -29432,13 +29610,13 @@
         <v>21</v>
       </c>
       <c r="B52" s="16" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C52" s="16" t="s">
         <v>1831</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="D52" s="16" t="s">
         <v>1832</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>1833</v>
       </c>
       <c r="E52" s="79"/>
       <c r="F52" s="79"/>
@@ -29453,13 +29631,13 @@
         <v>21</v>
       </c>
       <c r="B53" s="16" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>1834</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="D53" s="16" t="s">
         <v>1835</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>1836</v>
       </c>
       <c r="E53" s="79"/>
       <c r="F53" s="79"/>
@@ -29479,7 +29657,7 @@
         <v>1324</v>
       </c>
       <c r="B55" s="77" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="56">
@@ -29513,13 +29691,13 @@
         <v>21</v>
       </c>
       <c r="B57" s="16" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D57" s="16" t="s">
         <v>1838</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>1839</v>
       </c>
       <c r="E57" s="79"/>
       <c r="F57" s="79"/>
@@ -29534,13 +29712,13 @@
         <v>21</v>
       </c>
       <c r="B58" s="16" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D58" s="16" t="s">
         <v>1840</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>1840</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>1841</v>
       </c>
       <c r="E58" s="79"/>
       <c r="F58" s="79"/>
@@ -29555,13 +29733,13 @@
         <v>21</v>
       </c>
       <c r="B59" s="16" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D59" s="16" t="s">
         <v>1842</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>1842</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>1843</v>
       </c>
       <c r="E59" s="79"/>
       <c r="F59" s="79"/>
@@ -29576,13 +29754,13 @@
         <v>21</v>
       </c>
       <c r="B60" s="16" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>1844</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>1845</v>
       </c>
       <c r="E60" s="79"/>
       <c r="F60" s="79"/>
@@ -29597,13 +29775,13 @@
         <v>21</v>
       </c>
       <c r="B61" s="16" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D61" s="16" t="s">
         <v>1846</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>1846</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>1847</v>
       </c>
       <c r="E61" s="79"/>
       <c r="F61" s="79"/>
@@ -29618,13 +29796,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="16" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D62" s="16" t="s">
         <v>1848</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>1848</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>1849</v>
       </c>
       <c r="E62" s="79"/>
       <c r="F62" s="79"/>
@@ -29641,18 +29819,18 @@
     </row>
     <row r="64">
       <c r="A64" s="74" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B64" s="89" t="s">
-        <v>1850</v>
+        <v>1754</v>
+      </c>
+      <c r="B64" s="95" t="s">
+        <v>1849</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="74" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B65" s="90" t="s">
-        <v>1851</v>
+        <v>1756</v>
+      </c>
+      <c r="B65" s="96" t="s">
+        <v>1850</v>
       </c>
     </row>
     <row r="66">
@@ -29665,7 +29843,7 @@
         <v>1324</v>
       </c>
       <c r="B67" s="77" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="68">
@@ -29699,13 +29877,13 @@
         <v>21</v>
       </c>
       <c r="B69" s="16" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C69" s="16" t="s">
         <v>1853</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="D69" s="16" t="s">
         <v>1854</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>1855</v>
       </c>
       <c r="E69" s="79"/>
       <c r="F69" s="79"/>
@@ -29720,13 +29898,13 @@
         <v>21</v>
       </c>
       <c r="B70" s="16" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C70" s="16" t="s">
         <v>1856</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="D70" s="16" t="s">
         <v>1857</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>1858</v>
       </c>
       <c r="E70" s="79"/>
       <c r="F70" s="79"/>
@@ -29741,13 +29919,13 @@
         <v>21</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>1859</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="D71" s="16" t="s">
         <v>1860</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>1861</v>
       </c>
       <c r="E71" s="79"/>
       <c r="F71" s="79"/>
@@ -29762,13 +29940,13 @@
         <v>21</v>
       </c>
       <c r="B72" s="16" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>1862</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="D72" s="16" t="s">
         <v>1863</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>1864</v>
       </c>
       <c r="E72" s="79"/>
       <c r="F72" s="79"/>
@@ -29788,7 +29966,7 @@
         <v>1324</v>
       </c>
       <c r="B74" s="77" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="75">
@@ -29822,13 +30000,13 @@
         <v>21</v>
       </c>
       <c r="B76" s="16" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C76" s="16" t="s">
         <v>1866</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="D76" s="16" t="s">
         <v>1867</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>1868</v>
       </c>
       <c r="E76" s="79"/>
       <c r="F76" s="79"/>
@@ -29843,13 +30021,13 @@
         <v>21</v>
       </c>
       <c r="B77" s="16" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C77" s="16" t="s">
         <v>1869</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="D77" s="16" t="s">
         <v>1870</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>1871</v>
       </c>
       <c r="E77" s="79"/>
       <c r="F77" s="79"/>
@@ -29864,13 +30042,13 @@
         <v>21</v>
       </c>
       <c r="B78" s="16" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C78" s="16" t="s">
         <v>1872</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="D78" s="16" t="s">
         <v>1873</v>
-      </c>
-      <c r="D78" s="16" t="s">
-        <v>1874</v>
       </c>
       <c r="E78" s="79"/>
       <c r="F78" s="79"/>
@@ -29885,13 +30063,13 @@
         <v>21</v>
       </c>
       <c r="B79" s="16" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C79" s="16" t="s">
         <v>1875</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>1876</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>1877</v>
       </c>
       <c r="E79" s="79"/>
       <c r="F79" s="79"/>
@@ -29906,13 +30084,13 @@
         <v>21</v>
       </c>
       <c r="B80" s="16" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C80" s="16" t="s">
         <v>1878</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="D80" s="16" t="s">
         <v>1879</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>1880</v>
       </c>
       <c r="E80" s="79"/>
       <c r="F80" s="79"/>
@@ -29927,13 +30105,13 @@
         <v>21</v>
       </c>
       <c r="B81" s="16" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C81" s="16" t="s">
         <v>1881</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="D81" s="16" t="s">
         <v>1882</v>
-      </c>
-      <c r="D81" s="16" t="s">
-        <v>1883</v>
       </c>
       <c r="E81" s="79"/>
       <c r="F81" s="79"/>

</xml_diff>